<commit_message>
We already filter out priority demand changes with an effective day <= the start-day, so we don't want to call rest on those demand changes anymore.
</commit_message>
<xml_diff>
--- a/test-data/peak_hold_test-2-input.xlsx
+++ b/test-data/peak_hold_test-2-input.xlsx
@@ -11,6 +11,9 @@
     <sheet name="DemandRecords" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="SupplyRecords" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">DemandRecords!$A$1:$P$8</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -95,25 +98,25 @@
     <t xml:space="preserve">OI18</t>
   </si>
   <si>
+    <t xml:space="preserve">HLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT-AC-MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC_NonBOG-War</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cannibal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NonBOG-RC-Only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OffFORGE</t>
+  </si>
+  <si>
     <t xml:space="preserve">III Kruge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOT-AC-MIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC_NonBOG-War</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cannibal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NonBOG-RC-Only</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OffFORGE</t>
   </si>
   <si>
     <t xml:space="preserve">Component</t>
@@ -177,9 +180,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -289,7 +293,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -306,6 +310,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -334,7 +342,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -411,6 +419,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -418,11 +430,11 @@
   </sheetPr>
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.35"/>
@@ -461,7 +473,7 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
@@ -481,363 +493,364 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
+      <c r="A2" s="5" t="n">
         <v>67</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="7" t="n">
         <v>722</v>
       </c>
-      <c r="D2" s="6" t="n">
+      <c r="D2" s="7" t="n">
         <v>24</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="8" t="n">
+      <c r="K2" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="10" t="n">
-        <v>45</v>
-      </c>
-      <c r="N2" s="4" t="n">
+      <c r="M2" s="11" t="n">
+        <v>45</v>
+      </c>
+      <c r="N2" s="5" t="n">
         <v>10</v>
       </c>
       <c r="O2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="4" t="n">
+      <c r="P2" s="5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
-        <v>68</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" s="6" t="n">
-        <v>746</v>
-      </c>
-      <c r="D3" s="6" t="n">
-        <v>8</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="A3" s="5" t="n">
+        <v>70</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7" t="n">
+        <v>722</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>64</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="G3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="8" t="n">
+      <c r="K3" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="N3" s="0" t="n">
+      <c r="M3" s="11" t="n">
+        <v>45</v>
+      </c>
+      <c r="N3" s="5" t="n">
         <v>10</v>
       </c>
       <c r="O3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="4" t="n">
-        <v>2</v>
+      <c r="P3" s="5" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
-        <v>69</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="6" t="n">
-        <v>754</v>
-      </c>
-      <c r="D4" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="A4" s="5" t="n">
+        <v>70</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>722</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>64</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="8" t="n">
+      <c r="F4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="10" t="n">
-        <v>45</v>
-      </c>
-      <c r="N4" s="4" t="n">
+      <c r="M4" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="N4" s="0" t="n">
         <v>10</v>
       </c>
       <c r="O4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="4" t="n">
-        <v>3</v>
+      <c r="P4" s="5" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
+      <c r="A5" s="5" t="n">
         <v>70</v>
       </c>
-      <c r="B5" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" s="6" t="n">
-        <v>778</v>
-      </c>
-      <c r="D5" s="6" t="n">
-        <v>8</v>
-      </c>
-      <c r="E5" s="7" t="s">
+      <c r="B5" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>722</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>65</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="4" t="s">
+      <c r="G5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="8" t="n">
+      <c r="K5" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="N5" s="0" t="n">
+      <c r="M5" s="11" t="n">
+        <v>45</v>
+      </c>
+      <c r="N5" s="5" t="n">
         <v>10</v>
       </c>
       <c r="O5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="4" t="n">
-        <v>4</v>
+      <c r="P5" s="5" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="n">
-        <v>70</v>
-      </c>
-      <c r="B6" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="6" t="n">
-        <v>722</v>
-      </c>
-      <c r="D6" s="6" t="n">
-        <v>64</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="A6" s="5" t="n">
+        <v>68</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>746</v>
+      </c>
+      <c r="D6" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="4" t="s">
+      <c r="G6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="8" t="n">
+      <c r="K6" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="10" t="n">
-        <v>45</v>
-      </c>
-      <c r="N6" s="4" t="n">
+      <c r="M6" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="N6" s="0" t="n">
         <v>10</v>
       </c>
       <c r="O6" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="P6" s="4" t="n">
-        <v>5</v>
+      <c r="P6" s="5" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="n">
-        <v>70</v>
-      </c>
-      <c r="B7" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6" t="n">
-        <v>722</v>
-      </c>
-      <c r="D7" s="6" t="n">
-        <v>64</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="A7" s="5" t="n">
+        <v>69</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>754</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>24</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" s="8" t="n">
+      <c r="F7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="N7" s="0" t="n">
+      <c r="M7" s="11" t="n">
+        <v>45</v>
+      </c>
+      <c r="N7" s="5" t="n">
         <v>10</v>
       </c>
       <c r="O7" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="P7" s="4" t="n">
-        <v>6</v>
+      <c r="P7" s="5" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
+      <c r="A8" s="5" t="n">
         <v>70</v>
       </c>
-      <c r="B8" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="6" t="n">
-        <v>722</v>
-      </c>
-      <c r="D8" s="6" t="n">
-        <v>65</v>
-      </c>
-      <c r="E8" s="7" t="s">
+      <c r="B8" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>778</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="8" t="n">
+      <c r="K8" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="L8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="10" t="n">
-        <v>45</v>
-      </c>
-      <c r="N8" s="4" t="n">
+      <c r="M8" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="N8" s="0" t="n">
         <v>10</v>
       </c>
       <c r="O8" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="P8" s="4" t="n">
-        <v>7</v>
+      <c r="P8" s="5" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:P8"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -845,6 +858,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -856,10 +870,10 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.1"/>
@@ -880,220 +894,220 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="11" t="n">
+      <c r="B2" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="n">
+      <c r="C2" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="11" t="n">
+      <c r="G2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="J2" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="11" t="n">
+      <c r="J2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="M2" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="O2" s="11" t="s">
+      <c r="M2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="P2" s="11" t="n">
+      <c r="P2" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="Q2" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="11" t="n">
+      <c r="B3" s="12" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C3" s="11" t="n">
+      <c r="C3" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="11" t="n">
+      <c r="G3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="J3" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" s="11" t="n">
+      <c r="J3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="M3" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="O3" s="11" t="s">
+      <c r="M3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="P3" s="11" t="n">
+      <c r="P3" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="11" t="n">
+      <c r="B4" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C4" s="11" t="n">
+      <c r="C4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="11" t="n">
+      <c r="G4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="J4" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4" s="11" t="n">
+      <c r="J4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="M4" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="O4" s="11" t="s">
+      <c r="M4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="P4" s="11" t="n">
+      <c r="P4" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="Q4" s="4" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>